<commit_message>
Update sierra leone location data
</commit_message>
<xml_diff>
--- a/mosip_master/xlsx/zone.xlsx
+++ b/mosip_master/xlsx/zone.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20361"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MOSIP\Country Details\Seirra Leone\SLE_Master_Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MicroTech\IdeaProjects\mosip-data-sln\mosip_master\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BA16D6F-698E-46AC-A025-9B46DEB9EC1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B83AD60A-9D35-448D-A4BE-F4CBD457AA34}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{2D18BD18-8EBD-40B0-81ED-2940D035647B}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8940" xr2:uid="{2D18BD18-8EBD-40B0-81ED-2940D035647B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="77">
   <si>
     <t>lang_code</t>
   </si>
@@ -66,9 +66,6 @@
     <t>SOU</t>
   </si>
   <si>
-    <t>South</t>
-  </si>
-  <si>
     <t>Region</t>
   </si>
   <si>
@@ -78,9 +75,6 @@
     <t>EST</t>
   </si>
   <si>
-    <t>EAST</t>
-  </si>
-  <si>
     <t>SLE/EST</t>
   </si>
   <si>
@@ -129,64 +123,139 @@
     <t>SLE/EST/KEN</t>
   </si>
   <si>
-    <t>KAK</t>
-  </si>
-  <si>
-    <t>Kakua</t>
-  </si>
-  <si>
-    <t>Chiefdom</t>
-  </si>
-  <si>
-    <t>SLE/SOU/BO/KAK</t>
-  </si>
-  <si>
-    <t>NON</t>
-  </si>
-  <si>
-    <t>Nongowa</t>
-  </si>
-  <si>
-    <t>SLE/EST/KEN/NON</t>
-  </si>
-  <si>
-    <t>NSS</t>
-  </si>
-  <si>
-    <t>New Site Section</t>
-  </si>
-  <si>
-    <t>Section</t>
-  </si>
-  <si>
-    <t>SLE/SOU/BO/KAK/NSS</t>
-  </si>
-  <si>
-    <t>MES</t>
-  </si>
-  <si>
-    <t>Messima</t>
-  </si>
-  <si>
-    <t>SLE/SOU/BO/KAK/MES</t>
-  </si>
-  <si>
-    <t>LUM</t>
-  </si>
-  <si>
-    <t>Lumbebu</t>
-  </si>
-  <si>
-    <t>SLE/EST/KEN/NON/LUM</t>
-  </si>
-  <si>
-    <t>LAM</t>
-  </si>
-  <si>
-    <t>Lambayama</t>
-  </si>
-  <si>
-    <t>SLE/EST/KEN/NON/LAM</t>
+    <t>Southern</t>
+  </si>
+  <si>
+    <t>Eastern</t>
+  </si>
+  <si>
+    <t>NES</t>
+  </si>
+  <si>
+    <t>North East</t>
+  </si>
+  <si>
+    <t>SLE/NES</t>
+  </si>
+  <si>
+    <t>NWS</t>
+  </si>
+  <si>
+    <t>North West</t>
+  </si>
+  <si>
+    <t>SLE/NWS</t>
+  </si>
+  <si>
+    <t>WST</t>
+  </si>
+  <si>
+    <t>Western</t>
+  </si>
+  <si>
+    <t>SLE/WST</t>
+  </si>
+  <si>
+    <t>KAI</t>
+  </si>
+  <si>
+    <t>SLE/EST/KAI</t>
+  </si>
+  <si>
+    <t>KON</t>
+  </si>
+  <si>
+    <t>SLE/EST/KON</t>
+  </si>
+  <si>
+    <t>BOM</t>
+  </si>
+  <si>
+    <t>SLE/NES/BOM</t>
+  </si>
+  <si>
+    <t>FAL</t>
+  </si>
+  <si>
+    <t>SLE/NES/FAL</t>
+  </si>
+  <si>
+    <t>KOI</t>
+  </si>
+  <si>
+    <t>SLE/NES/KOI</t>
+  </si>
+  <si>
+    <t>TON</t>
+  </si>
+  <si>
+    <t>SLE/NES/TON</t>
+  </si>
+  <si>
+    <t>KAM</t>
+  </si>
+  <si>
+    <t>SLE/NWS/KAM</t>
+  </si>
+  <si>
+    <t>KAR</t>
+  </si>
+  <si>
+    <t>SLE/NWS/KAR</t>
+  </si>
+  <si>
+    <t>POR</t>
+  </si>
+  <si>
+    <t>SLE/NWS/POR</t>
+  </si>
+  <si>
+    <t>RUR</t>
+  </si>
+  <si>
+    <t>SLE/WST/RUR</t>
+  </si>
+  <si>
+    <t>URB</t>
+  </si>
+  <si>
+    <t>SLE/WST/URB</t>
+  </si>
+  <si>
+    <t>Kailahun</t>
+  </si>
+  <si>
+    <t>Kono</t>
+  </si>
+  <si>
+    <t>Bombali</t>
+  </si>
+  <si>
+    <t>Falaba</t>
+  </si>
+  <si>
+    <t>Koinadugu</t>
+  </si>
+  <si>
+    <t>Tonkolili</t>
+  </si>
+  <si>
+    <t>Kambia</t>
+  </si>
+  <si>
+    <t>Karene</t>
+  </si>
+  <si>
+    <t>Port Loko</t>
+  </si>
+  <si>
+    <t>Bo</t>
+  </si>
+  <si>
+    <t>Western Rural</t>
+  </si>
+  <si>
+    <t>Western Urban</t>
   </si>
 </sst>
 </file>
@@ -313,7 +382,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -323,12 +392,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -341,9 +404,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -660,7 +720,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -668,15 +728,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD87EAB5-0ECB-4730-9A7F-26273B58F35B}">
-  <dimension ref="A1:H15"/>
+  <dimension ref="A1:H23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:8" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:8" ht="42" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -702,365 +762,573 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="5">
+      <c r="D2" s="10">
         <v>0</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="6"/>
-      <c r="H2" s="7" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="8" t="s">
+      <c r="G2" s="4"/>
+      <c r="H2" s="5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="6" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="9" t="s">
         <v>12</v>
       </c>
       <c r="C3" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" s="10">
+        <v>1</v>
+      </c>
+      <c r="E3" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="10">
-        <v>1</v>
-      </c>
-      <c r="E3" s="9" t="s">
+      <c r="F3" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="9" t="s">
+      <c r="G3" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="H3" s="5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="G3" s="9" t="s">
+      <c r="C4" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D4" s="10">
+        <v>1</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G4" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="H3" s="7" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" s="12" t="s">
+      <c r="H4" s="5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="D5" s="10">
+        <v>1</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="H5" s="5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D6" s="10">
+        <v>1</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="H6" s="5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="D7" s="10">
+        <v>1</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="H7" s="5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="D8" s="10">
+        <v>2</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="H8" s="5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" s="10">
+        <v>2</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="H9" s="5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="D10" s="10">
+        <v>2</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="H10" s="5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="D11" s="10">
+        <v>2</v>
+      </c>
+      <c r="E11" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="H11" s="5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="D12" s="10">
+        <v>2</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="H12" s="5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="D13" s="10">
+        <v>2</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="G13" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="H13" s="5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="D14" s="10">
+        <v>2</v>
+      </c>
+      <c r="E14" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="F14" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="G14" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="H14" s="5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="D15" s="10">
+        <v>2</v>
+      </c>
+      <c r="E15" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="G15" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="H15" s="5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="D16" s="10">
+        <v>2</v>
+      </c>
+      <c r="E16" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="G16" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="H16" s="5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="D17" s="10">
+        <v>2</v>
+      </c>
+      <c r="E17" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="F17" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="G17" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="H17" s="5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B18" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="13">
-        <v>1</v>
-      </c>
-      <c r="E4" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="F4" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="G4" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="H4" s="7" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="12" t="s">
+      <c r="C18" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="D18" s="10">
+        <v>2</v>
+      </c>
+      <c r="E18" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="F18" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" s="13">
-        <v>2</v>
-      </c>
-      <c r="E5" s="12" t="s">
+      <c r="G18" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="H18" s="5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B19" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="F5" s="9" t="s">
+      <c r="C19" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="G5" s="9" t="s">
+      <c r="D19" s="10">
+        <v>2</v>
+      </c>
+      <c r="E19" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="F19" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="G19" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="H5" s="7" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="C6" s="12" t="s">
+      <c r="H19" s="5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B20" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="D6" s="13">
-        <v>2</v>
-      </c>
-      <c r="E6" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="F6" s="9" t="s">
+      <c r="C20" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="G6" s="9" t="s">
+      <c r="D20" s="10">
+        <v>2</v>
+      </c>
+      <c r="E20" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="F20" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="G20" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="H6" s="7" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="C7" s="12" t="s">
+      <c r="H20" s="5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B21" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="D7" s="13">
-        <v>2</v>
-      </c>
-      <c r="E7" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="F7" s="9" t="s">
+      <c r="C21" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="G7" s="9" t="s">
+      <c r="D21" s="10">
+        <v>2</v>
+      </c>
+      <c r="E21" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="F21" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="G21" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="H7" s="7" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="C8" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="D8" s="13">
-        <v>2</v>
-      </c>
-      <c r="E8" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="F8" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="G8" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="H8" s="7" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="C9" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="D9" s="13">
-        <v>2</v>
-      </c>
-      <c r="E9" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="F9" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="G9" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="H9" s="7" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="C10" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="D10" s="13">
-        <v>3</v>
-      </c>
-      <c r="E10" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="F10" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="G10" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="H10" s="7" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="B11" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="C11" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="D11" s="13">
-        <v>3</v>
-      </c>
-      <c r="E11" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="F11" s="9" t="s">
+      <c r="H21" s="5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B22" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="D22" s="10">
+        <v>2</v>
+      </c>
+      <c r="E22" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="F22" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="G22" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="G11" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="H11" s="7" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="40" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="B12" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="C12" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="D12" s="13">
-        <v>4</v>
-      </c>
-      <c r="E12" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="F12" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="G12" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="H12" s="7" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="40" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="B13" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="C13" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="D13" s="13">
-        <v>4</v>
-      </c>
-      <c r="E13" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="F13" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="G13" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="H13" s="7" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="40" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A14" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="B14" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="C14" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="D14" s="13">
-        <v>4</v>
-      </c>
-      <c r="E14" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="F14" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="G14" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="H14" s="7" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="40" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A15" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="B15" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="C15" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="D15" s="13">
-        <v>4</v>
-      </c>
-      <c r="E15" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="F15" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="G15" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="H15" s="7" t="b">
+      <c r="H22" s="5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B23" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="D23" s="10">
+        <v>2</v>
+      </c>
+      <c r="E23" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="F23" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="G23" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="H23" s="5" t="b">
         <v>1</v>
       </c>
     </row>

</xml_diff>